<commit_message>
KAI: Fixed second inversion bug
</commit_message>
<xml_diff>
--- a/AdjusterTool2/LeafAreas.xlsx
+++ b/AdjusterTool2/LeafAreas.xlsx
@@ -54,10 +54,10 @@
     <t xml:space="preserve">Cut Far</t>
   </si>
   <si>
-    <t xml:space="preserve">Original Length</t>
+    <t xml:space="preserve">Original_Length</t>
   </si>
   <si>
-    <t xml:space="preserve">Remaining Length</t>
+    <t xml:space="preserve">Remaining_Length</t>
   </si>
   <si>
     <t xml:space="preserve">DefoID</t>
@@ -446,11 +446,11 @@
   </sheetPr>
   <dimension ref="A1:L571"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A296" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G330" activeCellId="0" sqref="G330"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.32"/>
@@ -9945,10 +9945,10 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.02"/>
@@ -10359,7 +10359,7 @@
       <selection pane="topLeft" activeCell="G64" activeCellId="0" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.47"/>
@@ -14411,7 +14411,7 @@
       <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.6"/>
@@ -16602,7 +16602,7 @@
       <selection pane="topLeft" activeCell="N37" activeCellId="0" sqref="N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.35"/>
@@ -16696,7 +16696,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>

</xml_diff>